<commit_message>
Updated History of Present Illness FHIR mapping
</commit_message>
<xml_diff>
--- a/documents/eCR_R1.1_FHIR_Mapping_dstu2_v2.xlsx
+++ b/documents/eCR_R1.1_FHIR_Mapping_dstu2_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbashyam/git/eCRNow/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECA7D94-A3DB-4441-9B0A-B2CF30BA0B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3A73A9-C732-483C-9B6F-32AE0CB4B209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="32380" windowHeight="20060" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Queries" sheetId="2" r:id="rId1"/>
@@ -735,9 +735,6 @@
     <t>Encounter.participant.individual.Practitioner.identifier</t>
   </si>
   <si>
-    <t>Condition.text</t>
-  </si>
-  <si>
     <t>observation[templateId/root='2.16.840.1.113883.10.20.22.4.44']/id</t>
   </si>
   <si>
@@ -1198,6 +1195,9 @@
     <t xml:space="preserve">GET [base]/Encounter/id, GET [base]/Organization/id
 Encounter.serviceProvider - Organization
 </t>
+  </si>
+  <si>
+    <t>Condition.code.text</t>
   </si>
 </sst>
 </file>
@@ -1725,15 +1725,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="53.33203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="53.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="53.33203125" style="2"/>
+    <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="53.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1744,83 +1744,83 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B8" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>164</v>
       </c>
@@ -1828,18 +1828,18 @@
         <v>156</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>365</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -1852,29 +1852,29 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.83203125" style="24" customWidth="1"/>
-    <col min="11" max="11" width="26.5" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="16"/>
+    <col min="7" max="7" width="69.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.85546875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="19" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>102</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>63</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>95</v>
@@ -1906,10 +1906,10 @@
         <v>107</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
@@ -1941,21 +1941,21 @@
         <v>112</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>79</v>
@@ -1976,21 +1976,21 @@
         <v>112</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>93</v>
@@ -2011,21 +2011,21 @@
         <v>112</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>93</v>
@@ -2046,10 +2046,10 @@
         <v>112</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>140</v>
       </c>
@@ -2078,13 +2078,13 @@
         <v>80</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>140</v>
       </c>
@@ -2113,13 +2113,13 @@
         <v>80</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>140</v>
       </c>
@@ -2146,13 +2146,13 @@
         <v>92</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>140</v>
       </c>
@@ -2179,13 +2179,13 @@
         <v>92</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>140</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>168</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>92</v>
@@ -2212,13 +2212,13 @@
         <v>93</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>140</v>
       </c>
@@ -2245,13 +2245,13 @@
         <v>92</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>140</v>
       </c>
@@ -2278,13 +2278,13 @@
         <v>92</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>140</v>
       </c>
@@ -2311,13 +2311,13 @@
         <v>92</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>140</v>
       </c>
@@ -2344,13 +2344,13 @@
         <v>93</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>140</v>
       </c>
@@ -2379,13 +2379,13 @@
         <v>79</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>140</v>
       </c>
@@ -2411,16 +2411,16 @@
         <v>90</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>140</v>
       </c>
@@ -2449,13 +2449,13 @@
         <v>92</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>140</v>
       </c>
@@ -2484,13 +2484,13 @@
         <v>93</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>140</v>
       </c>
@@ -2519,13 +2519,13 @@
         <v>92</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>140</v>
       </c>
@@ -2554,13 +2554,13 @@
         <v>92</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>140</v>
       </c>
@@ -2587,13 +2587,13 @@
         <v>93</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>140</v>
       </c>
@@ -2620,13 +2620,13 @@
         <v>93</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>139</v>
       </c>
@@ -2653,13 +2653,13 @@
         <v>92</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>139</v>
       </c>
@@ -2684,13 +2684,13 @@
         <v>93</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>139</v>
       </c>
@@ -2715,13 +2715,13 @@
         <v>92</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>139</v>
       </c>
@@ -2746,13 +2746,13 @@
         <v>92</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>139</v>
       </c>
@@ -2777,13 +2777,13 @@
         <v>92</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>139</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>139</v>
       </c>
@@ -2839,13 +2839,13 @@
         <v>92</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>139</v>
       </c>
@@ -2870,13 +2870,13 @@
         <v>92</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>139</v>
       </c>
@@ -2901,13 +2901,13 @@
         <v>93</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>139</v>
       </c>
@@ -2932,13 +2932,13 @@
         <v>93</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>139</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>139</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>139</v>
       </c>
@@ -3025,47 +3025,47 @@
         <v>93</v>
       </c>
       <c r="J35" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>148</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="6" t="s">
         <v>138</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>149</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>168</v>
@@ -3080,18 +3080,18 @@
         <v>138</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>104</v>
       </c>
@@ -3118,13 +3118,13 @@
         <v>93</v>
       </c>
       <c r="J38" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>104</v>
       </c>
@@ -3142,18 +3142,18 @@
         <v>138</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>104</v>
       </c>
@@ -3180,13 +3180,13 @@
         <v>79</v>
       </c>
       <c r="J40" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>139</v>
       </c>
@@ -3211,13 +3211,13 @@
         <v>93</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>139</v>
       </c>
@@ -3242,13 +3242,13 @@
         <v>93</v>
       </c>
       <c r="J42" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>139</v>
       </c>
@@ -3273,13 +3273,13 @@
         <v>93</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>33</v>
       </c>
@@ -3299,20 +3299,20 @@
         <v>96</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>230</v>
+        <v>375</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J44" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>35</v>
       </c>
@@ -3332,20 +3332,20 @@
         <v>138</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J45" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>218</v>
       </c>
@@ -3372,24 +3372,24 @@
         <v>92</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>80</v>
@@ -3398,31 +3398,31 @@
         <v>138</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6" t="s">
         <v>92</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>93</v>
@@ -3431,31 +3431,31 @@
         <v>138</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6" t="s">
         <v>92</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>92</v>
@@ -3464,31 +3464,31 @@
         <v>138</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>92</v>
@@ -3497,31 +3497,31 @@
         <v>138</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>92</v>
@@ -3530,20 +3530,20 @@
         <v>138</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>218</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>179</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>79</v>
@@ -3573,21 +3573,21 @@
         <v>112</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>179</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>79</v>
@@ -3596,7 +3596,7 @@
         <v>138</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="s">
@@ -3606,21 +3606,21 @@
         <v>112</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>218</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>179</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>79</v>
@@ -3629,7 +3629,7 @@
         <v>138</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6" t="s">
@@ -3639,30 +3639,30 @@
         <v>112</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F55" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>90</v>
@@ -3671,33 +3671,33 @@
         <v>79</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>90</v>
@@ -3706,33 +3706,33 @@
         <v>79</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>90</v>
@@ -3741,33 +3741,33 @@
         <v>79</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>90</v>
@@ -3776,13 +3776,13 @@
         <v>79</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>106</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>178</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>79</v>
@@ -3802,7 +3802,7 @@
         <v>125</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>90</v>
@@ -3814,10 +3814,10 @@
         <v>131</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>106</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>185</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>79</v>
@@ -3837,7 +3837,7 @@
         <v>125</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>90</v>
@@ -3849,10 +3849,10 @@
         <v>131</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>106</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>184</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>79</v>
@@ -3872,7 +3872,7 @@
         <v>125</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>90</v>
@@ -3884,10 +3884,10 @@
         <v>131</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>106</v>
       </c>
@@ -3917,10 +3917,10 @@
         <v>131</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>106</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>184</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="6" t="s">
@@ -3948,10 +3948,10 @@
         <v>131</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>106</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>178</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>80</v>
@@ -3971,7 +3971,7 @@
         <v>125</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6" t="s">
@@ -3981,10 +3981,10 @@
         <v>131</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>106</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>185</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>80</v>
@@ -4004,7 +4004,7 @@
         <v>125</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6" t="s">
@@ -4014,21 +4014,21 @@
         <v>131</v>
       </c>
       <c r="K65" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>79</v>
@@ -4037,7 +4037,7 @@
         <v>125</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6" t="s">
@@ -4047,21 +4047,21 @@
         <v>131</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>92</v>
@@ -4070,7 +4070,7 @@
         <v>125</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6" t="s">
@@ -4080,21 +4080,21 @@
         <v>131</v>
       </c>
       <c r="K67" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>79</v>
@@ -4103,7 +4103,7 @@
         <v>125</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6" t="s">
@@ -4113,21 +4113,21 @@
         <v>131</v>
       </c>
       <c r="K68" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>92</v>
@@ -4136,7 +4136,7 @@
         <v>125</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6" t="s">
@@ -4146,21 +4146,21 @@
         <v>131</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>93</v>
@@ -4169,7 +4169,7 @@
         <v>125</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6" t="s">
@@ -4179,21 +4179,21 @@
         <v>131</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>93</v>
@@ -4202,7 +4202,7 @@
         <v>125</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6" t="s">
@@ -4212,21 +4212,21 @@
         <v>131</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>93</v>
@@ -4235,7 +4235,7 @@
         <v>125</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6" t="s">
@@ -4245,21 +4245,21 @@
         <v>131</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>92</v>
@@ -4268,7 +4268,7 @@
         <v>125</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6" t="s">
@@ -4278,10 +4278,10 @@
         <v>131</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>105</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>186</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>79</v>
@@ -4310,15 +4310,15 @@
         <v>79</v>
       </c>
       <c r="J74" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>100</v>
@@ -4345,13 +4345,13 @@
         <v>79</v>
       </c>
       <c r="J75" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>105</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>188</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>79</v>
@@ -4380,24 +4380,24 @@
         <v>79</v>
       </c>
       <c r="J76" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>186</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>79</v>
@@ -4406,20 +4406,20 @@
         <v>96</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6" t="s">
         <v>93</v>
       </c>
       <c r="J77" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>105</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>42</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>208</v>
@@ -4446,24 +4446,24 @@
         <v>93</v>
       </c>
       <c r="J78" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>79</v>
@@ -4479,13 +4479,13 @@
         <v>93</v>
       </c>
       <c r="J79" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>105</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>189</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>79</v>
@@ -4512,13 +4512,13 @@
         <v>93</v>
       </c>
       <c r="J80" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>105</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>189</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>79</v>
@@ -4545,13 +4545,13 @@
         <v>93</v>
       </c>
       <c r="J81" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>105</v>
       </c>
@@ -4562,25 +4562,25 @@
         <v>189</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="6" t="s">
         <v>96</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
       <c r="J82" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
         <v>165</v>
       </c>
@@ -4600,25 +4600,25 @@
         <v>138</v>
       </c>
       <c r="G83" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H83" s="11"/>
       <c r="I83" s="11" t="s">
         <v>79</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C84" s="17" t="s">
         <v>166</v>
@@ -4633,25 +4633,25 @@
         <v>138</v>
       </c>
       <c r="G84" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H84" s="11"/>
       <c r="I84" s="11" t="s">
         <v>92</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K84" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C85" s="17" t="s">
         <v>166</v>
@@ -4666,25 +4666,25 @@
         <v>138</v>
       </c>
       <c r="G85" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H85" s="11"/>
       <c r="I85" s="11" t="s">
         <v>79</v>
       </c>
       <c r="J85" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K85" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C86" s="17" t="s">
         <v>166</v>
@@ -4699,25 +4699,25 @@
         <v>138</v>
       </c>
       <c r="G86" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H86" s="11"/>
       <c r="I86" s="11" t="s">
         <v>79</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K86" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>166</v>
@@ -4732,25 +4732,25 @@
         <v>138</v>
       </c>
       <c r="G87" s="23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H87" s="11"/>
       <c r="I87" s="11" t="s">
         <v>93</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>166</v>
@@ -4765,25 +4765,25 @@
         <v>138</v>
       </c>
       <c r="G88" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H88" s="11"/>
       <c r="I88" s="11" t="s">
         <v>93</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K88" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C89" s="17" t="s">
         <v>166</v>
@@ -4798,20 +4798,20 @@
         <v>138</v>
       </c>
       <c r="G89" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H89" s="11"/>
       <c r="I89" s="11" t="s">
         <v>93</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K89" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>164</v>
       </c>
@@ -4843,10 +4843,10 @@
         <v>156</v>
       </c>
       <c r="K90" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>164</v>
       </c>
@@ -4878,10 +4878,10 @@
         <v>156</v>
       </c>
       <c r="K91" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>164</v>
       </c>
@@ -4913,10 +4913,10 @@
         <v>156</v>
       </c>
       <c r="K92" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>164</v>
       </c>
@@ -4948,10 +4948,10 @@
         <v>156</v>
       </c>
       <c r="K93" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>164</v>
       </c>
@@ -4981,10 +4981,10 @@
         <v>156</v>
       </c>
       <c r="K94" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>164</v>
       </c>
@@ -5016,10 +5016,10 @@
         <v>156</v>
       </c>
       <c r="K95" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>164</v>
       </c>
@@ -5049,10 +5049,10 @@
         <v>156</v>
       </c>
       <c r="K96" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>164</v>
       </c>
@@ -5082,10 +5082,10 @@
         <v>156</v>
       </c>
       <c r="K97" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>164</v>
       </c>
@@ -5117,10 +5117,10 @@
         <v>156</v>
       </c>
       <c r="K98" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>104</v>
       </c>
@@ -5140,18 +5140,18 @@
         <v>138</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
       <c r="J99" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K99" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>104</v>
       </c>
@@ -5171,18 +5171,18 @@
         <v>138</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H100" s="6"/>
       <c r="I100" s="6"/>
       <c r="J100" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K100" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>104</v>
       </c>
@@ -5202,18 +5202,18 @@
         <v>138</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
       <c r="J101" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K101" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>104</v>
       </c>
@@ -5233,15 +5233,15 @@
         <v>138</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
       <c r="J102" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K102" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5252,28 +5252,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAEF04E9A1B48544A813770D804417BF" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5f6564d6fd1be9d83e2a64915f5205a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e84ddf88720b63dcc3a8c6c9e2ce95b4" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5524,26 +5502,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F38DC35-61B7-4F0C-AF24-8F7D63AD6B02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5563,4 +5544,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>